<commit_message>
student upload template modified
</commit_message>
<xml_diff>
--- a/uploads/upload_templates/student_upload_template.xlsx
+++ b/uploads/upload_templates/student_upload_template.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\xampp\htdocs\projects\chm\uploads\upload_templates\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CFD5586-7D8A-47D4-B381-744E5FD2CB63}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="upload_data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -48,14 +42,14 @@
     <t>STATUS</t>
   </si>
   <si>
-    <t>STUDENT_ID</t>
+    <t>REGISTRATION NO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -194,7 +188,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -229,7 +223,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -406,21 +400,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
@@ -434,7 +428,7 @@
     <col min="10" max="10" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -454,7 +448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>

</xml_diff>